<commit_message>
Added images of the excel data and organized a bit
</commit_message>
<xml_diff>
--- a/MicroDepGraph/Opinions.xlsx
+++ b/MicroDepGraph/Opinions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\Universidad\SWME\SME-Group1\MicroDepGraph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD9F79B-1F90-4C15-95B5-1A4F807E5E5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F56AC1-735D-4EA8-AC82-92294B33B7C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -169,7 +169,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,8 +212,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -265,12 +271,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
+      <left style="medium">
         <color auto="1"/>
       </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thick">
         <color auto="1"/>
       </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thick">
         <color auto="1"/>
       </top>
@@ -281,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -298,7 +335,6 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -306,6 +342,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -314,6 +367,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0099FF"/>
+      <color rgb="FF00FF00"/>
+      <color rgb="FF963900"/>
       <color rgb="FF660066"/>
       <color rgb="FFFF99FF"/>
     </mruColors>
@@ -594,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,54 +667,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="11" t="s">
         <v>26</v>
       </c>
+      <c r="P1" s="19"/>
     </row>
     <row r="2" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
@@ -704,9 +761,10 @@
         <f>AVERAGE(B2:N2)</f>
         <v>2.5384615384615383</v>
       </c>
+      <c r="P2" s="19"/>
     </row>
     <row r="3" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2">
@@ -752,9 +810,10 @@
         <f t="shared" ref="O3:O13" si="0">AVERAGE(B3:N3)</f>
         <v>2.4615384615384617</v>
       </c>
+      <c r="P3" s="19"/>
     </row>
     <row r="4" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -800,9 +859,10 @@
         <f t="shared" si="0"/>
         <v>3.3076923076923075</v>
       </c>
+      <c r="P4" s="19"/>
     </row>
     <row r="5" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2">
@@ -848,9 +908,10 @@
         <f t="shared" si="0"/>
         <v>2.0769230769230771</v>
       </c>
+      <c r="P5" s="19"/>
     </row>
     <row r="6" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1">
@@ -896,9 +957,10 @@
         <f t="shared" si="0"/>
         <v>4.3076923076923075</v>
       </c>
+      <c r="P6" s="19"/>
     </row>
     <row r="7" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2">
@@ -944,9 +1006,10 @@
         <f t="shared" si="0"/>
         <v>2.1538461538461537</v>
       </c>
+      <c r="P7" s="19"/>
     </row>
     <row r="8" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1">
@@ -992,9 +1055,10 @@
         <f t="shared" si="0"/>
         <v>2.6153846153846154</v>
       </c>
+      <c r="P8" s="19"/>
     </row>
     <row r="9" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2">
@@ -1040,9 +1104,10 @@
         <f t="shared" si="0"/>
         <v>3.1538461538461537</v>
       </c>
+      <c r="P9" s="19"/>
     </row>
     <row r="10" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1">
@@ -1088,9 +1153,10 @@
         <f t="shared" si="0"/>
         <v>4.0769230769230766</v>
       </c>
+      <c r="P10" s="19"/>
     </row>
     <row r="11" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2">
@@ -1136,9 +1202,10 @@
         <f t="shared" si="0"/>
         <v>2.8461538461538463</v>
       </c>
+      <c r="P11" s="19"/>
     </row>
     <row r="12" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1">
@@ -1184,66 +1251,86 @@
         <f t="shared" si="0"/>
         <v>3.3846153846153846</v>
       </c>
+      <c r="P12" s="19"/>
     </row>
     <row r="13" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
-        <v>4</v>
-      </c>
-      <c r="C13" s="2">
-        <v>5</v>
-      </c>
-      <c r="D13" s="4">
-        <v>3</v>
-      </c>
-      <c r="E13" s="4">
-        <v>3</v>
-      </c>
-      <c r="F13" s="4">
-        <v>3</v>
-      </c>
-      <c r="G13" s="4">
-        <v>3</v>
-      </c>
-      <c r="H13" s="4">
-        <v>4</v>
-      </c>
-      <c r="I13" s="4">
-        <v>4</v>
-      </c>
-      <c r="J13" s="4">
-        <v>2</v>
-      </c>
-      <c r="K13" s="4">
-        <v>2</v>
-      </c>
-      <c r="L13" s="4">
-        <v>2</v>
-      </c>
-      <c r="M13" s="4">
-        <v>2</v>
-      </c>
-      <c r="N13" s="6">
-        <v>3</v>
-      </c>
-      <c r="O13" s="8">
+      <c r="B13" s="16">
+        <v>4</v>
+      </c>
+      <c r="C13" s="16">
+        <v>5</v>
+      </c>
+      <c r="D13" s="17">
+        <v>3</v>
+      </c>
+      <c r="E13" s="17">
+        <v>3</v>
+      </c>
+      <c r="F13" s="17">
+        <v>3</v>
+      </c>
+      <c r="G13" s="17">
+        <v>3</v>
+      </c>
+      <c r="H13" s="17">
+        <v>4</v>
+      </c>
+      <c r="I13" s="17">
+        <v>4</v>
+      </c>
+      <c r="J13" s="17">
+        <v>2</v>
+      </c>
+      <c r="K13" s="17">
+        <v>2</v>
+      </c>
+      <c r="L13" s="17">
+        <v>2</v>
+      </c>
+      <c r="M13" s="17">
+        <v>2</v>
+      </c>
+      <c r="N13" s="18">
+        <v>3</v>
+      </c>
+      <c r="O13" s="7">
         <f t="shared" si="0"/>
         <v>3.0769230769230771</v>
       </c>
+      <c r="P13" s="19"/>
     </row>
     <row r="14" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="21"/>
       <c r="O14" s="7">
         <f>AVERAGE(O2:O13)</f>
         <v>3</v>
       </c>
-      <c r="P14" s="15" t="s">
+      <c r="P14" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A14:N14"/>
+    <mergeCell ref="P1:P13"/>
+  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B2:N13">
     <cfRule type="colorScale" priority="2">

</xml_diff>

<commit_message>
Added images and part of visualization Readme
</commit_message>
<xml_diff>
--- a/MicroDepGraph/Opinions.xlsx
+++ b/MicroDepGraph/Opinions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\Universidad\SWME\SME-Group1\MicroDepGraph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F56AC1-735D-4EA8-AC82-92294B33B7C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8455C0F-7DD7-47D3-9CF5-69C073CDF25F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>PROJECTS NAME</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>TOTAL AVERAGE</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -350,13 +359,13 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -383,6 +392,972 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.4104017935258093"/>
+          <c:y val="0.19486111111111112"/>
+          <c:w val="0.55081342957130364"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>e-commerce-microservices-sample</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cqrs-microservice-sampler</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>data-services-javaee7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>e-ground-2019</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>empathy_delivery</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>LakesideMutual</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>lelylan</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Microservices-Demo</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>odm-ondocker</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>rsa</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>springboot-graphql-databases</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>spring-petclinic-microservices</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$2:$O$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2.5384615384615383</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4615384615384617</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3076923076923075</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0769230769230771</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.3076923076923075</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1538461538461537</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6153846153846154</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1538461538461537</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0769230769230766</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.8461538461538463</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.3846153846153846</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0769230769230771</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-46D7-47BD-92FE-55C71CF9208E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="115"/>
+        <c:overlap val="-20"/>
+        <c:axId val="1912079727"/>
+        <c:axId val="1912492207"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1912079727"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1912492207"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1912492207"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1912079727"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="222">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>7326</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>5862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>663086</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>7327</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE183332-96DA-4FF5-8342-7C4BFC3E699F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -651,7 +1626,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,7 +1687,7 @@
       <c r="O1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="19"/>
+      <c r="P1" s="21"/>
     </row>
     <row r="2" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
@@ -761,7 +1736,7 @@
         <f>AVERAGE(B2:N2)</f>
         <v>2.5384615384615383</v>
       </c>
-      <c r="P2" s="19"/>
+      <c r="P2" s="21"/>
     </row>
     <row r="3" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
@@ -810,7 +1785,7 @@
         <f t="shared" ref="O3:O13" si="0">AVERAGE(B3:N3)</f>
         <v>2.4615384615384617</v>
       </c>
-      <c r="P3" s="19"/>
+      <c r="P3" s="21"/>
     </row>
     <row r="4" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
@@ -859,7 +1834,7 @@
         <f t="shared" si="0"/>
         <v>3.3076923076923075</v>
       </c>
-      <c r="P4" s="19"/>
+      <c r="P4" s="21"/>
     </row>
     <row r="5" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
@@ -908,7 +1883,7 @@
         <f t="shared" si="0"/>
         <v>2.0769230769230771</v>
       </c>
-      <c r="P5" s="19"/>
+      <c r="P5" s="21"/>
     </row>
     <row r="6" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
@@ -957,7 +1932,7 @@
         <f t="shared" si="0"/>
         <v>4.3076923076923075</v>
       </c>
-      <c r="P6" s="19"/>
+      <c r="P6" s="21"/>
     </row>
     <row r="7" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
@@ -1006,7 +1981,7 @@
         <f t="shared" si="0"/>
         <v>2.1538461538461537</v>
       </c>
-      <c r="P7" s="19"/>
+      <c r="P7" s="21"/>
     </row>
     <row r="8" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
@@ -1055,7 +2030,7 @@
         <f t="shared" si="0"/>
         <v>2.6153846153846154</v>
       </c>
-      <c r="P8" s="19"/>
+      <c r="P8" s="21"/>
     </row>
     <row r="9" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
@@ -1104,7 +2079,7 @@
         <f t="shared" si="0"/>
         <v>3.1538461538461537</v>
       </c>
-      <c r="P9" s="19"/>
+      <c r="P9" s="21"/>
     </row>
     <row r="10" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
@@ -1153,7 +2128,7 @@
         <f t="shared" si="0"/>
         <v>4.0769230769230766</v>
       </c>
-      <c r="P10" s="19"/>
+      <c r="P10" s="21"/>
     </row>
     <row r="11" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
@@ -1202,7 +2177,7 @@
         <f t="shared" si="0"/>
         <v>2.8461538461538463</v>
       </c>
-      <c r="P11" s="19"/>
+      <c r="P11" s="21"/>
     </row>
     <row r="12" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
@@ -1251,7 +2226,7 @@
         <f t="shared" si="0"/>
         <v>3.3846153846153846</v>
       </c>
-      <c r="P12" s="19"/>
+      <c r="P12" s="21"/>
     </row>
     <row r="13" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
@@ -1300,23 +2275,23 @@
         <f t="shared" si="0"/>
         <v>3.0769230769230771</v>
       </c>
-      <c r="P13" s="19"/>
+      <c r="P13" s="21"/>
     </row>
     <row r="14" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="21"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="20"/>
       <c r="O14" s="7">
         <f>AVERAGE(O2:O13)</f>
         <v>3</v>
@@ -1360,6 +2335,7 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>

</xml_diff>